<commit_message>
adapted costs of solar pv in mech turk
</commit_message>
<xml_diff>
--- a/scripts/query_generator/cost_update/cost_inputs.xlsx
+++ b/scripts/query_generator/cost_update/cost_inputs.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="29005"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10116"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kruip/Projects/mechanical_turk/scripts/query_generator/cost_update/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/martlubben/Projects/mechanical_turk/scripts/query_generator/cost_update/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="51200" windowHeight="27260" tabRatio="500" activeTab="13"/>
+    <workbookView xWindow="0" yWindow="440" windowWidth="28800" windowHeight="16320" tabRatio="500" activeTab="14" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="20131125" sheetId="7" r:id="rId1"/>
@@ -26,6 +26,7 @@
     <sheet name="20150817" sheetId="12" r:id="rId12"/>
     <sheet name="20171220" sheetId="13" r:id="rId13"/>
     <sheet name="20180103" sheetId="14" r:id="rId14"/>
+    <sheet name="20180302" sheetId="15" r:id="rId15"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">'20121221'!$A$1:$B$116</definedName>
@@ -39,7 +40,7 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">Sheet1!$A$1:$B$131</definedName>
     <definedName name="_xlnm.Extract" localSheetId="8">'20140725'!#REF!</definedName>
   </definedNames>
-  <calcPr calcId="140000" concurrentCalc="0"/>
+  <calcPr calcId="140000" calcOnSave="0"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -52,7 +53,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1817" uniqueCount="224">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1965" uniqueCount="224">
   <si>
     <t>key</t>
   </si>
@@ -729,7 +730,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -993,6 +994,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -1319,7 +1323,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B125"/>
   <sheetViews>
     <sheetView topLeftCell="A79" workbookViewId="0">
@@ -2337,7 +2341,7 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <dimension ref="A1:B121"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -3325,7 +3329,7 @@
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
   <dimension ref="A1:B121"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -4313,10 +4317,12 @@
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
   <dimension ref="A1:B121"/>
   <sheetViews>
-    <sheetView topLeftCell="A23" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
@@ -5300,10 +5306,10 @@
 </file>
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
   <dimension ref="A1:B152"/>
   <sheetViews>
-    <sheetView topLeftCell="A21" workbookViewId="0">
+    <sheetView topLeftCell="A73" workbookViewId="0">
       <selection activeCell="A161" sqref="A161"/>
     </sheetView>
   </sheetViews>
@@ -6530,7 +6536,7 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:B152">
+  <autoFilter ref="A1:B152" xr:uid="{00000000-0009-0000-0000-00000C000000}">
     <sortState ref="A2:B188">
       <sortCondition ref="B1:B188"/>
     </sortState>
@@ -6543,11 +6549,11 @@
 </file>
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0D00-000000000000}">
   <dimension ref="A1:B148"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:XFD1"/>
+    <sheetView topLeftCell="A124" workbookViewId="0">
+      <selection sqref="A1:B148"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -6558,570 +6564,570 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>68</v>
+        <v>44</v>
       </c>
       <c r="B1">
-        <v>14.7</v>
+        <v>292951.01382177602</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>185</v>
+        <v>45</v>
       </c>
       <c r="B2">
-        <v>21.588666666666601</v>
+        <v>206557.979478889</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>59</v>
+        <v>46</v>
       </c>
       <c r="B3">
-        <v>26</v>
+        <v>522419.90108401002</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>69</v>
+        <v>160</v>
       </c>
       <c r="B4">
-        <v>95.55</v>
+        <v>1691150.70153317</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>67</v>
+        <v>161</v>
       </c>
       <c r="B5">
-        <v>106.76404394968201</v>
+        <v>377953.62892607</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>36</v>
+        <v>167</v>
       </c>
       <c r="B6">
-        <v>152.4992</v>
+        <v>2622810</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>99</v>
+        <v>91</v>
       </c>
       <c r="B7">
-        <v>181</v>
+        <v>793333.33333333302</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>51</v>
+        <v>92</v>
       </c>
       <c r="B8">
-        <v>195.75</v>
+        <v>404644.32235354203</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>176</v>
+        <v>170</v>
       </c>
       <c r="B9">
-        <v>199</v>
+        <v>1691150.70153317</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>63</v>
+        <v>166</v>
       </c>
       <c r="B10">
-        <v>253.919603088467</v>
+        <v>481528.54067728599</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>55</v>
+        <v>29</v>
       </c>
       <c r="B11">
-        <v>288.12014659142898</v>
+        <v>2730510</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>56</v>
+        <v>97</v>
       </c>
       <c r="B12">
-        <v>355.89660019843001</v>
+        <v>287417.48431020498</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>60</v>
+        <v>176</v>
       </c>
       <c r="B13">
-        <v>368.24875718132301</v>
+        <v>199</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>57</v>
+        <v>94</v>
       </c>
       <c r="B14">
-        <v>458.65972536618602</v>
+        <v>1314033.7881918801</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>49</v>
+        <v>95</v>
       </c>
       <c r="B15">
-        <v>594.33333333333303</v>
+        <v>716744.54719699698</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>65</v>
+        <v>50</v>
       </c>
       <c r="B16">
-        <v>594.33333333333303</v>
+        <v>587333.33333333302</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>58</v>
+        <v>35</v>
       </c>
       <c r="B17">
-        <v>594.33333333333303</v>
+        <v>1735.4880000000001</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>66</v>
+        <v>47</v>
       </c>
       <c r="B18">
-        <v>633.33333333333303</v>
+        <v>4163.7757729998502</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>217</v>
+        <v>96</v>
       </c>
       <c r="B19">
-        <v>659.14177410719503</v>
+        <v>365365.4375</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>216</v>
+        <v>48</v>
       </c>
       <c r="B20">
-        <v>670.95293642180002</v>
+        <v>5267.5612080599603</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>61</v>
+        <v>49</v>
       </c>
       <c r="B21">
-        <v>762.37510679081004</v>
+        <v>594.33333333333303</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>220</v>
+        <v>51</v>
       </c>
       <c r="B22">
-        <v>857.71199999999999</v>
+        <v>195.75</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="B23">
-        <v>923.33333333333303</v>
+        <v>551905.197104141</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>110</v>
+        <v>52</v>
       </c>
       <c r="B24">
-        <v>933.33333333333303</v>
+        <v>1426.72034096074</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>108</v>
+        <v>53</v>
       </c>
       <c r="B25">
-        <v>933.33333333333303</v>
+        <v>13387.5</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>102</v>
+        <v>54</v>
       </c>
       <c r="B26">
-        <v>1031.35466666666</v>
+        <v>9684.2023494634104</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>106</v>
+        <v>219</v>
       </c>
       <c r="B27">
-        <v>1053.3306250000001</v>
+        <v>246255</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>101</v>
+        <v>215</v>
       </c>
       <c r="B28">
-        <v>1226.6666666666599</v>
+        <v>4187622.7828787998</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>103</v>
+        <v>154</v>
       </c>
       <c r="B29">
-        <v>1334.6880000000001</v>
+        <v>12516068.502366301</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>107</v>
+        <v>168</v>
       </c>
       <c r="B30">
-        <v>1356.62929166666</v>
+        <v>19245000</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>52</v>
+        <v>3</v>
       </c>
       <c r="B31">
-        <v>1426.72034096074</v>
+        <v>206419387.62367401</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>35</v>
+        <v>165</v>
       </c>
       <c r="B32">
-        <v>1735.4880000000001</v>
+        <v>135592935.27812499</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>124</v>
+        <v>4</v>
       </c>
       <c r="B33">
-        <v>1999.2794019999999</v>
+        <v>129225833.333333</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>125</v>
+        <v>221</v>
       </c>
       <c r="B34">
-        <v>1999.2794019999999</v>
+        <v>49491.780702923097</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>17</v>
+        <v>159</v>
       </c>
       <c r="B35">
-        <v>2453.3333333333298</v>
+        <v>4187622.7828787998</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>47</v>
+        <v>84</v>
       </c>
       <c r="B36">
-        <v>4163.7757729998502</v>
+        <v>3954160.8593265899</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>48</v>
+        <v>85</v>
       </c>
       <c r="B37">
-        <v>5267.5612080599603</v>
+        <v>6438179.4473842699</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>135</v>
+        <v>86</v>
       </c>
       <c r="B38">
-        <v>7789.1925490000003</v>
+        <v>793333.33333333302</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>54</v>
+        <v>87</v>
       </c>
       <c r="B39">
-        <v>9684.2023494634104</v>
+        <v>100225</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>53</v>
+        <v>88</v>
       </c>
       <c r="B40">
-        <v>13387.5</v>
+        <v>4920081.7629607096</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>37</v>
+        <v>89</v>
       </c>
       <c r="B41">
-        <v>34000</v>
+        <v>40000</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="B42">
-        <v>40000</v>
+        <v>9943749.0421455894</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>221</v>
+        <v>5</v>
       </c>
       <c r="B43">
-        <v>49491.780702923097</v>
+        <v>178999173.98829699</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>136</v>
+        <v>155</v>
       </c>
       <c r="B44">
-        <v>86884.467919999996</v>
+        <v>76566794.296346307</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>87</v>
+        <v>6</v>
       </c>
       <c r="B45">
-        <v>100225</v>
+        <v>157393563.666666</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>162</v>
+        <v>156</v>
       </c>
       <c r="B46">
-        <v>126253.64353350599</v>
+        <v>152735077.29472801</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
-        <v>195</v>
+        <v>37</v>
       </c>
       <c r="B47">
-        <v>173333.33333333299</v>
+        <v>34000</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
-        <v>81</v>
+        <v>178</v>
       </c>
       <c r="B48">
-        <v>206557.979478889</v>
+        <v>26320000</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
       <c r="B49">
-        <v>206557.979478889</v>
+        <v>15969915.2575</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
-        <v>218</v>
+        <v>138</v>
       </c>
       <c r="B50">
-        <v>246255</v>
+        <v>47926596.969999999</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
-        <v>219</v>
+        <v>39</v>
       </c>
       <c r="B51">
-        <v>246255</v>
+        <v>51155234.429589003</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
-        <v>97</v>
+        <v>40</v>
       </c>
       <c r="B52">
-        <v>287417.48431020498</v>
+        <v>3000000</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
-        <v>105</v>
+        <v>124</v>
       </c>
       <c r="B53">
-        <v>287417.48431020498</v>
+        <v>1999.2794019999999</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
-        <v>80</v>
+        <v>135</v>
       </c>
       <c r="B54">
-        <v>292951.01382177602</v>
+        <v>7789.1925490000003</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
-        <v>44</v>
+        <v>136</v>
       </c>
       <c r="B55">
-        <v>292951.01382177602</v>
+        <v>86884.467919999996</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
-        <v>137</v>
+        <v>24</v>
       </c>
       <c r="B56">
-        <v>321203.81650000002</v>
+        <v>389718771.83409399</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
-        <v>96</v>
+        <v>25</v>
       </c>
       <c r="B57">
-        <v>365365.4375</v>
+        <v>552526594.77124095</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
-        <v>161</v>
+        <v>41</v>
       </c>
       <c r="B58">
-        <v>377953.62892607</v>
+        <v>15172516.666666601</v>
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
-        <v>186</v>
+        <v>42</v>
       </c>
       <c r="B59">
-        <v>400000</v>
+        <v>1605000</v>
       </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
-        <v>187</v>
+        <v>7</v>
       </c>
       <c r="B60">
-        <v>400000</v>
+        <v>178439119.513818</v>
       </c>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
-        <v>188</v>
+        <v>43</v>
       </c>
       <c r="B61">
-        <v>400000</v>
+        <v>27456175</v>
       </c>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
-        <v>202</v>
+        <v>125</v>
       </c>
       <c r="B62">
-        <v>400000</v>
+        <v>1999.2794019999999</v>
       </c>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
-        <v>92</v>
+        <v>137</v>
       </c>
       <c r="B63">
-        <v>404644.32235354203</v>
+        <v>321203.81650000002</v>
       </c>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
-        <v>193</v>
+        <v>22</v>
       </c>
       <c r="B64">
-        <v>454750</v>
+        <v>6634766.74125</v>
       </c>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
-        <v>205</v>
+        <v>8</v>
       </c>
       <c r="B65">
-        <v>454750</v>
+        <v>137557916.73517799</v>
       </c>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
-        <v>214</v>
+        <v>9</v>
       </c>
       <c r="B66">
-        <v>454750</v>
+        <v>184005277.75251701</v>
       </c>
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="B67">
-        <v>481528.54067728599</v>
+        <v>117461956.55625001</v>
       </c>
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
-        <v>109</v>
+        <v>14</v>
       </c>
       <c r="B68">
-        <v>481528.54067728599</v>
+        <v>49359622.369231403</v>
       </c>
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
-        <v>82</v>
+        <v>10</v>
       </c>
       <c r="B69">
-        <v>522419.90108401002</v>
+        <v>112037800</v>
       </c>
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
-        <v>46</v>
+        <v>157</v>
       </c>
       <c r="B70">
-        <v>522419.90108401002</v>
+        <v>29085600</v>
       </c>
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
-        <v>27</v>
+        <v>11</v>
       </c>
       <c r="B71">
-        <v>531768.44999999995</v>
+        <v>240498185.091364</v>
       </c>
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.2">
@@ -7134,279 +7140,279 @@
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
-        <v>98</v>
+        <v>27</v>
       </c>
       <c r="B73">
-        <v>551905.197104141</v>
+        <v>531768.44999999995</v>
       </c>
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
-        <v>50</v>
+        <v>28</v>
       </c>
       <c r="B74">
-        <v>587333.33333333302</v>
+        <v>1643536.0106001699</v>
       </c>
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
-        <v>95</v>
+        <v>171</v>
       </c>
       <c r="B75">
-        <v>716744.54719699698</v>
+        <v>1691150.70153317</v>
       </c>
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
-        <v>91</v>
+        <v>109</v>
       </c>
       <c r="B76">
-        <v>793333.33333333302</v>
+        <v>481528.54067728599</v>
       </c>
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
-        <v>86</v>
+        <v>30</v>
       </c>
       <c r="B77">
-        <v>793333.33333333302</v>
+        <v>2730510</v>
       </c>
     </row>
     <row r="78" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
-        <v>192</v>
+        <v>105</v>
       </c>
       <c r="B78">
-        <v>893566.66666666605</v>
+        <v>287417.48431020498</v>
       </c>
     </row>
     <row r="79" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
-        <v>94</v>
+        <v>99</v>
       </c>
       <c r="B79">
-        <v>1314033.7881918801</v>
+        <v>181</v>
       </c>
     </row>
     <row r="80" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
-        <v>42</v>
+        <v>100</v>
       </c>
       <c r="B80">
-        <v>1605000</v>
+        <v>923.33333333333303</v>
       </c>
     </row>
     <row r="81" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
-        <v>28</v>
+        <v>101</v>
       </c>
       <c r="B81">
-        <v>1643536.0106001699</v>
+        <v>1226.6666666666599</v>
       </c>
     </row>
     <row r="82" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
-        <v>170</v>
+        <v>185</v>
       </c>
       <c r="B82">
-        <v>1691150.70153317</v>
+        <v>21.588666666666601</v>
       </c>
     </row>
     <row r="83" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
-        <v>171</v>
+        <v>220</v>
       </c>
       <c r="B83">
-        <v>1691150.70153317</v>
+        <v>857.71199999999999</v>
       </c>
     </row>
     <row r="84" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
-        <v>160</v>
+        <v>66</v>
       </c>
       <c r="B84">
-        <v>1691150.70153317</v>
+        <v>633.33333333333303</v>
       </c>
     </row>
     <row r="85" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
-        <v>167</v>
+        <v>36</v>
       </c>
       <c r="B85">
-        <v>2622810</v>
+        <v>152.4992</v>
       </c>
     </row>
     <row r="86" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
-        <v>29</v>
+        <v>55</v>
       </c>
       <c r="B86">
-        <v>2730510</v>
+        <v>288.12014659142898</v>
       </c>
     </row>
     <row r="87" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
-        <v>30</v>
+        <v>56</v>
       </c>
       <c r="B87">
-        <v>2730510</v>
+        <v>355.89660019843001</v>
       </c>
     </row>
     <row r="88" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
-        <v>40</v>
+        <v>57</v>
       </c>
       <c r="B88">
-        <v>3000000</v>
+        <v>458.65972536618602</v>
       </c>
     </row>
     <row r="89" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
-        <v>175</v>
+        <v>58</v>
       </c>
       <c r="B89">
-        <v>3002037.1384576601</v>
+        <v>594.33333333333303</v>
       </c>
     </row>
     <row r="90" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
-        <v>174</v>
+        <v>59</v>
       </c>
       <c r="B90">
-        <v>3430413.6215515998</v>
+        <v>26</v>
       </c>
     </row>
     <row r="91" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
-        <v>194</v>
+        <v>102</v>
       </c>
       <c r="B91">
-        <v>3802855.8845050498</v>
+        <v>1031.35466666666</v>
       </c>
     </row>
     <row r="92" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
-        <v>199</v>
+        <v>103</v>
       </c>
       <c r="B92">
-        <v>3802855.8845050498</v>
+        <v>1334.6880000000001</v>
       </c>
     </row>
     <row r="93" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
-        <v>201</v>
+        <v>217</v>
       </c>
       <c r="B93">
-        <v>3802855.8845050498</v>
+        <v>659.14177410719503</v>
       </c>
     </row>
     <row r="94" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
-        <v>207</v>
+        <v>108</v>
       </c>
       <c r="B94">
-        <v>3802855.8845050498</v>
+        <v>933.33333333333303</v>
       </c>
     </row>
     <row r="95" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
-        <v>209</v>
+        <v>60</v>
       </c>
       <c r="B95">
-        <v>3802855.8845050498</v>
+        <v>368.24875718132301</v>
       </c>
     </row>
     <row r="96" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
-        <v>79</v>
+        <v>61</v>
       </c>
       <c r="B96">
-        <v>3802855.8845050498</v>
+        <v>762.37510679081004</v>
       </c>
     </row>
     <row r="97" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
-        <v>84</v>
+        <v>63</v>
       </c>
       <c r="B97">
-        <v>3954160.8593265899</v>
+        <v>253.919603088467</v>
       </c>
     </row>
     <row r="98" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
-        <v>2</v>
+        <v>65</v>
       </c>
       <c r="B98">
-        <v>3973416.3049789998</v>
+        <v>594.33333333333303</v>
       </c>
     </row>
     <row r="99" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
-        <v>172</v>
+        <v>17</v>
       </c>
       <c r="B99">
-        <v>4187622.7828787998</v>
+        <v>2453.3333333333298</v>
       </c>
     </row>
     <row r="100" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
-        <v>190</v>
+        <v>106</v>
       </c>
       <c r="B100">
-        <v>4187622.7828787998</v>
+        <v>1053.3306250000001</v>
       </c>
     </row>
     <row r="101" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
-        <v>197</v>
+        <v>107</v>
       </c>
       <c r="B101">
-        <v>4187622.7828787998</v>
+        <v>1356.62929166666</v>
       </c>
     </row>
     <row r="102" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
-        <v>206</v>
+        <v>216</v>
       </c>
       <c r="B102">
-        <v>4187622.7828787998</v>
+        <v>670.95293642180002</v>
       </c>
     </row>
     <row r="103" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A103" t="s">
-        <v>208</v>
+        <v>110</v>
       </c>
       <c r="B103">
-        <v>4187622.7828787998</v>
+        <v>933.33333333333303</v>
       </c>
     </row>
     <row r="104" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A104" t="s">
-        <v>213</v>
+        <v>67</v>
       </c>
       <c r="B104">
-        <v>4187622.7828787998</v>
+        <v>106.76404394968201</v>
       </c>
     </row>
     <row r="105" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A105" t="s">
-        <v>173</v>
+        <v>68</v>
       </c>
       <c r="B105">
-        <v>4187622.7828787998</v>
+        <v>14.7</v>
       </c>
     </row>
     <row r="106" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A106" t="s">
-        <v>215</v>
+        <v>69</v>
       </c>
       <c r="B106">
-        <v>4187622.7828787998</v>
+        <v>95.55</v>
       </c>
     </row>
     <row r="107" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A107" t="s">
-        <v>159</v>
+        <v>173</v>
       </c>
       <c r="B107">
         <v>4187622.7828787998</v>
@@ -7414,15 +7420,15 @@
     </row>
     <row r="108" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A108" t="s">
-        <v>88</v>
+        <v>209</v>
       </c>
       <c r="B108">
-        <v>4920081.7629607096</v>
+        <v>3802855.8845050498</v>
       </c>
     </row>
     <row r="109" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A109" t="s">
-        <v>191</v>
+        <v>211</v>
       </c>
       <c r="B109">
         <v>5690950.8459237004</v>
@@ -7430,31 +7436,31 @@
     </row>
     <row r="110" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A110" t="s">
-        <v>196</v>
+        <v>208</v>
       </c>
       <c r="B110">
-        <v>5690950.8459237004</v>
+        <v>4187622.7828787998</v>
       </c>
     </row>
     <row r="111" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A111" t="s">
-        <v>198</v>
+        <v>210</v>
       </c>
       <c r="B111">
-        <v>5690950.8459237004</v>
+        <v>10056288.611111101</v>
       </c>
     </row>
     <row r="112" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A112" t="s">
-        <v>203</v>
+        <v>194</v>
       </c>
       <c r="B112">
-        <v>5690950.8459237004</v>
+        <v>3802855.8845050498</v>
       </c>
     </row>
     <row r="113" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A113" t="s">
-        <v>211</v>
+        <v>196</v>
       </c>
       <c r="B113">
         <v>5690950.8459237004</v>
@@ -7462,291 +7468,1498 @@
     </row>
     <row r="114" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A114" t="s">
-        <v>85</v>
+        <v>213</v>
       </c>
       <c r="B114">
-        <v>6438179.4473842699</v>
+        <v>4187622.7828787998</v>
       </c>
     </row>
     <row r="115" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A115" t="s">
-        <v>22</v>
+        <v>212</v>
       </c>
       <c r="B115">
-        <v>6634766.74125</v>
+        <v>10056288.611111101</v>
       </c>
     </row>
     <row r="116" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A116" t="s">
-        <v>90</v>
+        <v>186</v>
       </c>
       <c r="B116">
-        <v>9943749.0421455894</v>
+        <v>400000</v>
       </c>
     </row>
     <row r="117" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A117" t="s">
-        <v>189</v>
+        <v>193</v>
       </c>
       <c r="B117">
-        <v>10056288.611111101</v>
+        <v>454750</v>
       </c>
     </row>
     <row r="118" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A118" t="s">
-        <v>200</v>
+        <v>195</v>
       </c>
       <c r="B118">
-        <v>10056288.611111101</v>
+        <v>173333.33333333299</v>
       </c>
     </row>
     <row r="119" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A119" t="s">
-        <v>204</v>
+        <v>192</v>
       </c>
       <c r="B119">
-        <v>10056288.611111101</v>
+        <v>893566.66666666605</v>
       </c>
     </row>
     <row r="120" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A120" t="s">
-        <v>210</v>
+        <v>199</v>
       </c>
       <c r="B120">
-        <v>10056288.611111101</v>
+        <v>3802855.8845050498</v>
       </c>
     </row>
     <row r="121" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A121" t="s">
-        <v>212</v>
+        <v>198</v>
       </c>
       <c r="B121">
-        <v>10056288.611111101</v>
+        <v>5690950.8459237004</v>
       </c>
     </row>
     <row r="122" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A122" t="s">
-        <v>163</v>
+        <v>197</v>
       </c>
       <c r="B122">
-        <v>10344280.3994176</v>
+        <v>4187622.7828787998</v>
       </c>
     </row>
     <row r="123" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A123" t="s">
-        <v>154</v>
+        <v>200</v>
       </c>
       <c r="B123">
-        <v>12516068.502366301</v>
+        <v>10056288.611111101</v>
       </c>
     </row>
     <row r="124" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A124" t="s">
-        <v>41</v>
+        <v>187</v>
       </c>
       <c r="B124">
-        <v>15172516.666666601</v>
+        <v>400000</v>
       </c>
     </row>
     <row r="125" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A125" t="s">
-        <v>38</v>
+        <v>12</v>
       </c>
       <c r="B125">
-        <v>15969915.2575</v>
+        <v>17041164.819520399</v>
       </c>
     </row>
     <row r="126" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A126" t="s">
-        <v>12</v>
+        <v>162</v>
       </c>
       <c r="B126">
-        <v>17041164.819520399</v>
+        <v>126253.64353350599</v>
       </c>
     </row>
     <row r="127" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A127" t="s">
-        <v>168</v>
+        <v>163</v>
       </c>
       <c r="B127">
-        <v>19245000</v>
+        <v>10344280.3994176</v>
       </c>
     </row>
     <row r="128" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A128" t="s">
-        <v>178</v>
+        <v>2</v>
       </c>
       <c r="B128">
-        <v>26320000</v>
+        <v>3973416.3049789998</v>
       </c>
     </row>
     <row r="129" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A129" t="s">
-        <v>43</v>
+        <v>218</v>
       </c>
       <c r="B129">
-        <v>27456175</v>
+        <v>246255</v>
       </c>
     </row>
     <row r="130" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A130" t="s">
-        <v>157</v>
+        <v>201</v>
       </c>
       <c r="B130">
-        <v>29085600</v>
+        <v>3802855.8845050498</v>
       </c>
     </row>
     <row r="131" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A131" t="s">
-        <v>138</v>
+        <v>191</v>
       </c>
       <c r="B131">
-        <v>47926596.969999999</v>
+        <v>5690950.8459237004</v>
       </c>
     </row>
     <row r="132" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A132" t="s">
-        <v>14</v>
+        <v>190</v>
       </c>
       <c r="B132">
-        <v>49359622.369231403</v>
+        <v>4187622.7828787998</v>
       </c>
     </row>
     <row r="133" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A133" t="s">
-        <v>39</v>
+        <v>189</v>
       </c>
       <c r="B133">
-        <v>51155234.429589003</v>
+        <v>10056288.611111101</v>
       </c>
     </row>
     <row r="134" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A134" t="s">
-        <v>155</v>
+        <v>188</v>
       </c>
       <c r="B134">
-        <v>76566794.296346307</v>
+        <v>400000</v>
       </c>
     </row>
     <row r="135" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A135" t="s">
-        <v>10</v>
+        <v>214</v>
       </c>
       <c r="B135">
-        <v>112037800</v>
+        <v>454750</v>
       </c>
     </row>
     <row r="136" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A136" t="s">
-        <v>164</v>
+        <v>175</v>
       </c>
       <c r="B136">
-        <v>117461956.55625001</v>
+        <v>3002037.1384576601</v>
       </c>
     </row>
     <row r="137" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A137" t="s">
-        <v>4</v>
+        <v>207</v>
       </c>
       <c r="B137">
-        <v>129225833.333333</v>
+        <v>3802855.8845050498</v>
       </c>
     </row>
     <row r="138" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A138" t="s">
-        <v>165</v>
+        <v>203</v>
       </c>
       <c r="B138">
-        <v>135592935.27812499</v>
+        <v>5690950.8459237004</v>
       </c>
     </row>
     <row r="139" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A139" t="s">
-        <v>8</v>
+        <v>206</v>
       </c>
       <c r="B139">
-        <v>137557916.73517799</v>
+        <v>4187622.7828787998</v>
       </c>
     </row>
     <row r="140" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A140" t="s">
-        <v>156</v>
+        <v>204</v>
       </c>
       <c r="B140">
-        <v>152735077.29472801</v>
+        <v>10056288.611111101</v>
       </c>
     </row>
     <row r="141" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A141" t="s">
-        <v>6</v>
+        <v>202</v>
       </c>
       <c r="B141">
-        <v>157393563.666666</v>
+        <v>400000</v>
       </c>
     </row>
     <row r="142" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A142" t="s">
-        <v>7</v>
+        <v>205</v>
       </c>
       <c r="B142">
-        <v>178439119.513818</v>
+        <v>454750</v>
       </c>
     </row>
     <row r="143" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A143" t="s">
-        <v>5</v>
+        <v>174</v>
       </c>
       <c r="B143">
-        <v>178999173.98829699</v>
+        <v>3430413.6215515998</v>
       </c>
     </row>
     <row r="144" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A144" t="s">
-        <v>9</v>
+        <v>172</v>
       </c>
       <c r="B144">
-        <v>184005277.75251701</v>
+        <v>4187622.7828787998</v>
       </c>
     </row>
     <row r="145" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A145" t="s">
-        <v>3</v>
+        <v>79</v>
       </c>
       <c r="B145">
-        <v>206419387.62367401</v>
+        <v>3802855.8845050498</v>
       </c>
     </row>
     <row r="146" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A146" t="s">
-        <v>11</v>
+        <v>80</v>
       </c>
       <c r="B146">
-        <v>240498185.091364</v>
+        <v>292951.01382177602</v>
       </c>
     </row>
     <row r="147" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A147" t="s">
-        <v>24</v>
+        <v>81</v>
       </c>
       <c r="B147">
-        <v>389718771.83409399</v>
+        <v>206557.979478889</v>
       </c>
     </row>
     <row r="148" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A148" t="s">
-        <v>25</v>
+        <v>82</v>
       </c>
       <c r="B148">
-        <v>552526594.77124095</v>
+        <v>522419.90108401002</v>
       </c>
     </row>
   </sheetData>
+  <sortState ref="A1:B148">
+    <sortCondition ref="A1"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{29A1E198-E744-0F45-8483-AA87E5830D61}">
+  <dimension ref="A1:B148"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A75" workbookViewId="0">
+      <selection activeCell="F88" sqref="F88"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="36.33203125" customWidth="1"/>
+    <col min="2" max="2" width="31.33203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B1">
+        <v>292951.01382177602</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>45</v>
+      </c>
+      <c r="B2">
+        <v>206557.979478889</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>46</v>
+      </c>
+      <c r="B3">
+        <v>522419.90108401002</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>160</v>
+      </c>
+      <c r="B4">
+        <v>1691150.70153317</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>161</v>
+      </c>
+      <c r="B5">
+        <v>377953.62892607</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>167</v>
+      </c>
+      <c r="B6">
+        <v>2622810</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>91</v>
+      </c>
+      <c r="B7">
+        <v>793333.33333333302</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>92</v>
+      </c>
+      <c r="B8">
+        <v>404644.32235354203</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>170</v>
+      </c>
+      <c r="B9">
+        <v>1691150.70153317</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>166</v>
+      </c>
+      <c r="B10">
+        <v>481528.54067728599</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>29</v>
+      </c>
+      <c r="B11">
+        <v>2730510</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>97</v>
+      </c>
+      <c r="B12">
+        <v>287417.48431020498</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>176</v>
+      </c>
+      <c r="B13">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>94</v>
+      </c>
+      <c r="B14">
+        <v>1314033.7881918801</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>95</v>
+      </c>
+      <c r="B15">
+        <v>716744.54719699698</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>50</v>
+      </c>
+      <c r="B16">
+        <v>587333.33333333302</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>35</v>
+      </c>
+      <c r="B17">
+        <v>25.920984480000001</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>47</v>
+      </c>
+      <c r="B18">
+        <v>4163.7757729998502</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>96</v>
+      </c>
+      <c r="B19">
+        <v>365365.4375</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>48</v>
+      </c>
+      <c r="B20">
+        <v>5267.5612080599603</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>49</v>
+      </c>
+      <c r="B21">
+        <v>594.33333333333303</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>51</v>
+      </c>
+      <c r="B22">
+        <v>195.75</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>98</v>
+      </c>
+      <c r="B23">
+        <v>551905.197104141</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>52</v>
+      </c>
+      <c r="B24">
+        <v>1426.72034096074</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>53</v>
+      </c>
+      <c r="B25">
+        <v>13387.5</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>54</v>
+      </c>
+      <c r="B26">
+        <v>9684.2023494634104</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>219</v>
+      </c>
+      <c r="B27">
+        <v>246255</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
+        <v>215</v>
+      </c>
+      <c r="B28">
+        <v>4187622.7828787998</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
+        <v>154</v>
+      </c>
+      <c r="B29">
+        <v>12516068.502366301</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
+        <v>168</v>
+      </c>
+      <c r="B30">
+        <v>19245000</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A31" t="s">
+        <v>3</v>
+      </c>
+      <c r="B31">
+        <v>206419387.62367401</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A32" t="s">
+        <v>165</v>
+      </c>
+      <c r="B32">
+        <v>135592935.27812499</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A33" t="s">
+        <v>4</v>
+      </c>
+      <c r="B33">
+        <v>129225833.333333</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A34" t="s">
+        <v>221</v>
+      </c>
+      <c r="B34">
+        <v>49491.780702923097</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A35" t="s">
+        <v>159</v>
+      </c>
+      <c r="B35">
+        <v>4187622.7828787998</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A36" t="s">
+        <v>84</v>
+      </c>
+      <c r="B36">
+        <v>3954160.8593265899</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A37" t="s">
+        <v>85</v>
+      </c>
+      <c r="B37">
+        <v>6438179.4473842699</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A38" t="s">
+        <v>86</v>
+      </c>
+      <c r="B38">
+        <v>793333.33333333302</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A39" t="s">
+        <v>87</v>
+      </c>
+      <c r="B39">
+        <v>100225</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A40" t="s">
+        <v>88</v>
+      </c>
+      <c r="B40">
+        <v>4920081.7629607096</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A41" t="s">
+        <v>89</v>
+      </c>
+      <c r="B41">
+        <v>40000</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A42" t="s">
+        <v>90</v>
+      </c>
+      <c r="B42">
+        <v>9943749.0421455894</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A43" t="s">
+        <v>5</v>
+      </c>
+      <c r="B43">
+        <v>178999173.98829699</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A44" t="s">
+        <v>155</v>
+      </c>
+      <c r="B44">
+        <v>76566794.296346307</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A45" t="s">
+        <v>6</v>
+      </c>
+      <c r="B45">
+        <v>157393563.666666</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A46" t="s">
+        <v>156</v>
+      </c>
+      <c r="B46">
+        <v>152735077.29472801</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A47" t="s">
+        <v>37</v>
+      </c>
+      <c r="B47">
+        <v>34000</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A48" t="s">
+        <v>178</v>
+      </c>
+      <c r="B48">
+        <v>26320000</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A49" t="s">
+        <v>38</v>
+      </c>
+      <c r="B49">
+        <v>15969915.2575</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A50" t="s">
+        <v>138</v>
+      </c>
+      <c r="B50">
+        <v>47926596.969999999</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A51" t="s">
+        <v>39</v>
+      </c>
+      <c r="B51">
+        <v>51155234.429589003</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A52" t="s">
+        <v>40</v>
+      </c>
+      <c r="B52">
+        <v>3000000</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A53" t="s">
+        <v>124</v>
+      </c>
+      <c r="B53">
+        <v>1999.2794019999999</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A54" t="s">
+        <v>135</v>
+      </c>
+      <c r="B54">
+        <v>7789.1925490000003</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A55" t="s">
+        <v>136</v>
+      </c>
+      <c r="B55">
+        <v>86884.467919999996</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A56" t="s">
+        <v>24</v>
+      </c>
+      <c r="B56">
+        <v>389718771.83409399</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A57" t="s">
+        <v>25</v>
+      </c>
+      <c r="B57">
+        <v>552526594.77124095</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A58" t="s">
+        <v>41</v>
+      </c>
+      <c r="B58">
+        <v>15172516.666666601</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A59" t="s">
+        <v>42</v>
+      </c>
+      <c r="B59">
+        <v>1605000</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A60" t="s">
+        <v>7</v>
+      </c>
+      <c r="B60">
+        <v>178439119.513818</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A61" t="s">
+        <v>43</v>
+      </c>
+      <c r="B61">
+        <v>27456175</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A62" t="s">
+        <v>125</v>
+      </c>
+      <c r="B62">
+        <v>1999.2794019999999</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A63" t="s">
+        <v>137</v>
+      </c>
+      <c r="B63">
+        <v>321203.81650000002</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A64" t="s">
+        <v>22</v>
+      </c>
+      <c r="B64">
+        <v>6634766.74125</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A65" t="s">
+        <v>8</v>
+      </c>
+      <c r="B65">
+        <v>137557916.73517799</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A66" t="s">
+        <v>9</v>
+      </c>
+      <c r="B66">
+        <v>184005277.75251701</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A67" t="s">
+        <v>164</v>
+      </c>
+      <c r="B67">
+        <v>117461956.55625001</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A68" t="s">
+        <v>14</v>
+      </c>
+      <c r="B68">
+        <v>49359622.369231403</v>
+      </c>
+    </row>
+    <row r="69" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A69" t="s">
+        <v>10</v>
+      </c>
+      <c r="B69">
+        <v>112037800</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A70" t="s">
+        <v>157</v>
+      </c>
+      <c r="B70">
+        <v>29085600</v>
+      </c>
+    </row>
+    <row r="71" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A71" t="s">
+        <v>11</v>
+      </c>
+      <c r="B71">
+        <v>240498185.091364</v>
+      </c>
+    </row>
+    <row r="72" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A72" t="s">
+        <v>26</v>
+      </c>
+      <c r="B72">
+        <v>531768.44999999995</v>
+      </c>
+    </row>
+    <row r="73" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A73" t="s">
+        <v>27</v>
+      </c>
+      <c r="B73">
+        <v>531768.44999999995</v>
+      </c>
+    </row>
+    <row r="74" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A74" t="s">
+        <v>28</v>
+      </c>
+      <c r="B74">
+        <v>1643536.0106001699</v>
+      </c>
+    </row>
+    <row r="75" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A75" t="s">
+        <v>171</v>
+      </c>
+      <c r="B75">
+        <v>1691150.70153317</v>
+      </c>
+    </row>
+    <row r="76" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A76" t="s">
+        <v>109</v>
+      </c>
+      <c r="B76">
+        <v>481528.54067728599</v>
+      </c>
+    </row>
+    <row r="77" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A77" t="s">
+        <v>30</v>
+      </c>
+      <c r="B77">
+        <v>2730510</v>
+      </c>
+    </row>
+    <row r="78" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A78" t="s">
+        <v>105</v>
+      </c>
+      <c r="B78">
+        <v>287417.48431020498</v>
+      </c>
+    </row>
+    <row r="79" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A79" t="s">
+        <v>99</v>
+      </c>
+      <c r="B79">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="80" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A80" t="s">
+        <v>100</v>
+      </c>
+      <c r="B80">
+        <v>923.33333333333303</v>
+      </c>
+    </row>
+    <row r="81" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A81" t="s">
+        <v>101</v>
+      </c>
+      <c r="B81">
+        <v>1226.6666666666599</v>
+      </c>
+    </row>
+    <row r="82" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A82" t="s">
+        <v>185</v>
+      </c>
+      <c r="B82">
+        <v>21.588666666666601</v>
+      </c>
+    </row>
+    <row r="83" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A83" t="s">
+        <v>220</v>
+      </c>
+      <c r="B83">
+        <v>857.71199999999999</v>
+      </c>
+    </row>
+    <row r="84" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A84" t="s">
+        <v>66</v>
+      </c>
+      <c r="B84">
+        <v>633.33333333333303</v>
+      </c>
+    </row>
+    <row r="85" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A85" t="s">
+        <v>36</v>
+      </c>
+      <c r="B85">
+        <v>25.920984480000001</v>
+      </c>
+    </row>
+    <row r="86" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A86" t="s">
+        <v>55</v>
+      </c>
+      <c r="B86">
+        <v>288.12014659142898</v>
+      </c>
+    </row>
+    <row r="87" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A87" t="s">
+        <v>56</v>
+      </c>
+      <c r="B87">
+        <v>355.89660019843001</v>
+      </c>
+    </row>
+    <row r="88" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A88" t="s">
+        <v>57</v>
+      </c>
+      <c r="B88">
+        <v>458.65972536618602</v>
+      </c>
+    </row>
+    <row r="89" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A89" t="s">
+        <v>58</v>
+      </c>
+      <c r="B89">
+        <v>594.33333333333303</v>
+      </c>
+    </row>
+    <row r="90" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A90" t="s">
+        <v>59</v>
+      </c>
+      <c r="B90">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="91" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A91" t="s">
+        <v>102</v>
+      </c>
+      <c r="B91">
+        <v>1031.35466666666</v>
+      </c>
+    </row>
+    <row r="92" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A92" t="s">
+        <v>103</v>
+      </c>
+      <c r="B92">
+        <v>1334.6880000000001</v>
+      </c>
+    </row>
+    <row r="93" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A93" t="s">
+        <v>217</v>
+      </c>
+      <c r="B93">
+        <v>659.14177410719503</v>
+      </c>
+    </row>
+    <row r="94" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A94" t="s">
+        <v>108</v>
+      </c>
+      <c r="B94">
+        <v>933.33333333333303</v>
+      </c>
+    </row>
+    <row r="95" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A95" t="s">
+        <v>60</v>
+      </c>
+      <c r="B95">
+        <v>368.24875718132301</v>
+      </c>
+    </row>
+    <row r="96" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A96" t="s">
+        <v>61</v>
+      </c>
+      <c r="B96">
+        <v>762.37510679081004</v>
+      </c>
+    </row>
+    <row r="97" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A97" t="s">
+        <v>63</v>
+      </c>
+      <c r="B97">
+        <v>253.919603088467</v>
+      </c>
+    </row>
+    <row r="98" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A98" t="s">
+        <v>65</v>
+      </c>
+      <c r="B98">
+        <v>594.33333333333303</v>
+      </c>
+    </row>
+    <row r="99" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A99" t="s">
+        <v>17</v>
+      </c>
+      <c r="B99">
+        <v>2453.3333333333298</v>
+      </c>
+    </row>
+    <row r="100" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A100" t="s">
+        <v>106</v>
+      </c>
+      <c r="B100">
+        <v>1053.3306250000001</v>
+      </c>
+    </row>
+    <row r="101" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A101" t="s">
+        <v>107</v>
+      </c>
+      <c r="B101">
+        <v>1356.62929166666</v>
+      </c>
+    </row>
+    <row r="102" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A102" t="s">
+        <v>216</v>
+      </c>
+      <c r="B102">
+        <v>670.95293642180002</v>
+      </c>
+    </row>
+    <row r="103" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A103" t="s">
+        <v>110</v>
+      </c>
+      <c r="B103">
+        <v>933.33333333333303</v>
+      </c>
+    </row>
+    <row r="104" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A104" t="s">
+        <v>67</v>
+      </c>
+      <c r="B104">
+        <v>106.76404394968201</v>
+      </c>
+    </row>
+    <row r="105" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A105" t="s">
+        <v>68</v>
+      </c>
+      <c r="B105">
+        <v>14.7</v>
+      </c>
+    </row>
+    <row r="106" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A106" t="s">
+        <v>69</v>
+      </c>
+      <c r="B106">
+        <v>95.55</v>
+      </c>
+    </row>
+    <row r="107" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A107" t="s">
+        <v>173</v>
+      </c>
+      <c r="B107">
+        <v>4187622.7828787998</v>
+      </c>
+    </row>
+    <row r="108" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A108" t="s">
+        <v>209</v>
+      </c>
+      <c r="B108">
+        <v>3802855.8845050498</v>
+      </c>
+    </row>
+    <row r="109" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A109" t="s">
+        <v>211</v>
+      </c>
+      <c r="B109">
+        <v>5690950.8459237004</v>
+      </c>
+    </row>
+    <row r="110" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A110" t="s">
+        <v>208</v>
+      </c>
+      <c r="B110">
+        <v>4187622.7828787998</v>
+      </c>
+    </row>
+    <row r="111" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A111" t="s">
+        <v>210</v>
+      </c>
+      <c r="B111">
+        <v>10056288.611111101</v>
+      </c>
+    </row>
+    <row r="112" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A112" t="s">
+        <v>194</v>
+      </c>
+      <c r="B112">
+        <v>3802855.8845050498</v>
+      </c>
+    </row>
+    <row r="113" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A113" t="s">
+        <v>196</v>
+      </c>
+      <c r="B113">
+        <v>5690950.8459237004</v>
+      </c>
+    </row>
+    <row r="114" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A114" t="s">
+        <v>213</v>
+      </c>
+      <c r="B114">
+        <v>4187622.7828787998</v>
+      </c>
+    </row>
+    <row r="115" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A115" t="s">
+        <v>212</v>
+      </c>
+      <c r="B115">
+        <v>10056288.611111101</v>
+      </c>
+    </row>
+    <row r="116" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A116" t="s">
+        <v>186</v>
+      </c>
+      <c r="B116">
+        <v>400000</v>
+      </c>
+    </row>
+    <row r="117" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A117" t="s">
+        <v>193</v>
+      </c>
+      <c r="B117">
+        <v>454750</v>
+      </c>
+    </row>
+    <row r="118" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A118" t="s">
+        <v>195</v>
+      </c>
+      <c r="B118">
+        <v>173333.33333333299</v>
+      </c>
+    </row>
+    <row r="119" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A119" t="s">
+        <v>192</v>
+      </c>
+      <c r="B119">
+        <v>893566.66666666605</v>
+      </c>
+    </row>
+    <row r="120" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A120" t="s">
+        <v>199</v>
+      </c>
+      <c r="B120">
+        <v>3802855.8845050498</v>
+      </c>
+    </row>
+    <row r="121" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A121" t="s">
+        <v>198</v>
+      </c>
+      <c r="B121">
+        <v>5690950.8459237004</v>
+      </c>
+    </row>
+    <row r="122" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A122" t="s">
+        <v>197</v>
+      </c>
+      <c r="B122">
+        <v>4187622.7828787998</v>
+      </c>
+    </row>
+    <row r="123" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A123" t="s">
+        <v>200</v>
+      </c>
+      <c r="B123">
+        <v>10056288.611111101</v>
+      </c>
+    </row>
+    <row r="124" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A124" t="s">
+        <v>187</v>
+      </c>
+      <c r="B124">
+        <v>400000</v>
+      </c>
+    </row>
+    <row r="125" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A125" t="s">
+        <v>12</v>
+      </c>
+      <c r="B125">
+        <v>17041164.819520399</v>
+      </c>
+    </row>
+    <row r="126" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A126" t="s">
+        <v>162</v>
+      </c>
+      <c r="B126">
+        <v>126253.64353350599</v>
+      </c>
+    </row>
+    <row r="127" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A127" t="s">
+        <v>163</v>
+      </c>
+      <c r="B127">
+        <v>10344280.3994176</v>
+      </c>
+    </row>
+    <row r="128" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A128" t="s">
+        <v>2</v>
+      </c>
+      <c r="B128">
+        <v>3973416.3049789998</v>
+      </c>
+    </row>
+    <row r="129" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A129" t="s">
+        <v>218</v>
+      </c>
+      <c r="B129">
+        <v>246255</v>
+      </c>
+    </row>
+    <row r="130" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A130" t="s">
+        <v>201</v>
+      </c>
+      <c r="B130">
+        <v>3802855.8845050498</v>
+      </c>
+    </row>
+    <row r="131" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A131" t="s">
+        <v>191</v>
+      </c>
+      <c r="B131">
+        <v>5690950.8459237004</v>
+      </c>
+    </row>
+    <row r="132" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A132" t="s">
+        <v>190</v>
+      </c>
+      <c r="B132">
+        <v>4187622.7828787998</v>
+      </c>
+    </row>
+    <row r="133" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A133" t="s">
+        <v>189</v>
+      </c>
+      <c r="B133">
+        <v>10056288.611111101</v>
+      </c>
+    </row>
+    <row r="134" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A134" t="s">
+        <v>188</v>
+      </c>
+      <c r="B134">
+        <v>400000</v>
+      </c>
+    </row>
+    <row r="135" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A135" t="s">
+        <v>214</v>
+      </c>
+      <c r="B135">
+        <v>454750</v>
+      </c>
+    </row>
+    <row r="136" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A136" t="s">
+        <v>175</v>
+      </c>
+      <c r="B136">
+        <v>3002037.1384576601</v>
+      </c>
+    </row>
+    <row r="137" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A137" t="s">
+        <v>207</v>
+      </c>
+      <c r="B137">
+        <v>3802855.8845050498</v>
+      </c>
+    </row>
+    <row r="138" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A138" t="s">
+        <v>203</v>
+      </c>
+      <c r="B138">
+        <v>5690950.8459237004</v>
+      </c>
+    </row>
+    <row r="139" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A139" t="s">
+        <v>206</v>
+      </c>
+      <c r="B139">
+        <v>4187622.7828787998</v>
+      </c>
+    </row>
+    <row r="140" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A140" t="s">
+        <v>204</v>
+      </c>
+      <c r="B140">
+        <v>10056288.611111101</v>
+      </c>
+    </row>
+    <row r="141" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A141" t="s">
+        <v>202</v>
+      </c>
+      <c r="B141">
+        <v>400000</v>
+      </c>
+    </row>
+    <row r="142" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A142" t="s">
+        <v>205</v>
+      </c>
+      <c r="B142">
+        <v>454750</v>
+      </c>
+    </row>
+    <row r="143" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A143" t="s">
+        <v>174</v>
+      </c>
+      <c r="B143">
+        <v>3430413.6215515998</v>
+      </c>
+    </row>
+    <row r="144" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A144" t="s">
+        <v>172</v>
+      </c>
+      <c r="B144">
+        <v>4187622.7828787998</v>
+      </c>
+    </row>
+    <row r="145" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A145" t="s">
+        <v>79</v>
+      </c>
+      <c r="B145">
+        <v>3802855.8845050498</v>
+      </c>
+    </row>
+    <row r="146" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A146" t="s">
+        <v>80</v>
+      </c>
+      <c r="B146">
+        <v>292951.01382177602</v>
+      </c>
+    </row>
+    <row r="147" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A147" t="s">
+        <v>81</v>
+      </c>
+      <c r="B147">
+        <v>206557.979478889</v>
+      </c>
+    </row>
+    <row r="148" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A148" t="s">
+        <v>82</v>
+      </c>
+      <c r="B148">
+        <v>522419.90108401002</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:B50"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -8164,7 +9377,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:B168"/>
   <sheetViews>
     <sheetView topLeftCell="A121" workbookViewId="0">
@@ -9452,7 +10665,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:B118"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -10410,7 +11623,7 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:B118">
+  <autoFilter ref="A1:B118" xr:uid="{00000000-0009-0000-0000-000003000000}">
     <sortState ref="A2:B118">
       <sortCondition ref="A1:A118"/>
     </sortState>
@@ -10420,7 +11633,7 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:B116"/>
   <sheetViews>
     <sheetView topLeftCell="A98" workbookViewId="0">
@@ -11368,7 +12581,7 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:B131"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -12430,7 +13643,7 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:B131">
+  <autoFilter ref="A1:B131" xr:uid="{00000000-0009-0000-0000-000005000000}">
     <sortState ref="A2:B131">
       <sortCondition ref="A1:A131"/>
     </sortState>
@@ -12441,7 +13654,7 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:F156"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -13689,7 +14902,7 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:B145"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -14870,7 +16083,7 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:B120"/>
   <sheetViews>
     <sheetView topLeftCell="A86" workbookViewId="0">

</xml_diff>

<commit_message>
New files for costs_specs.rb
</commit_message>
<xml_diff>
--- a/scripts/query_generator/cost_update/cost_inputs.xlsx
+++ b/scripts/query_generator/cost_update/cost_inputs.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10116"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10523"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/martlubben/Projects/mechanical_turk/scripts/query_generator/cost_update/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/marliekeverweij/Projects/mechanical_turk/scripts/query_generator/cost_update/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B6DEE0F-4890-AB49-A29A-46962449989A}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="440" windowWidth="28800" windowHeight="16320" tabRatio="500" activeTab="14" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="26800" tabRatio="500" firstSheet="3" activeTab="15" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="20131125" sheetId="7" r:id="rId1"/>
@@ -27,6 +28,7 @@
     <sheet name="20171220" sheetId="13" r:id="rId13"/>
     <sheet name="20180103" sheetId="14" r:id="rId14"/>
     <sheet name="20180302" sheetId="15" r:id="rId15"/>
+    <sheet name="20180612" sheetId="16" r:id="rId16"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">'20121221'!$A$1:$B$116</definedName>
@@ -36,11 +38,12 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="8" hidden="1">'20140725'!$A$1:$B$120</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="12" hidden="1">'20171220'!$A$1:$B$152</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="13" hidden="1">'20180103'!#REF!</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="15" hidden="1">'20180612'!$A$1:$B$153</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="9" hidden="1">Blad1!$A$1:$B$121</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">Sheet1!$A$1:$B$131</definedName>
     <definedName name="_xlnm.Extract" localSheetId="8">'20140725'!#REF!</definedName>
   </definedNames>
-  <calcPr calcId="140000" calcOnSave="0"/>
+  <calcPr calcId="140000"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -53,7 +56,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1965" uniqueCount="224">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2119" uniqueCount="237">
   <si>
     <t>key</t>
   </si>
@@ -725,6 +728,45 @@
   </si>
   <si>
     <t>transport_car_using_hydrogen</t>
+  </si>
+  <si>
+    <t>energy_power_turbine_hydrogen</t>
+  </si>
+  <si>
+    <t>agriculture_burner_hydrogen</t>
+  </si>
+  <si>
+    <t>households_collective_burner_network_gas</t>
+  </si>
+  <si>
+    <t>households_collective_heatpump_water_water_electricity</t>
+  </si>
+  <si>
+    <t>households_collective_burner_hydrogen</t>
+  </si>
+  <si>
+    <t>buildings_collective_burner_hydrogen</t>
+  </si>
+  <si>
+    <t>buildings_collective_burner_network_gas</t>
+  </si>
+  <si>
+    <t>buildings_collective_heatpump_water_water_electricity</t>
+  </si>
+  <si>
+    <t>industry_chemicals_refineries_burner_hydrogen</t>
+  </si>
+  <si>
+    <t>industry_other_paper_burner_hydrogen</t>
+  </si>
+  <si>
+    <t>industry_other_food_burner_hydrogen</t>
+  </si>
+  <si>
+    <t>industry_chemicals_fertilizers_burner_hydrogen</t>
+  </si>
+  <si>
+    <t>industry_chemicals_other_burner_hydrogen</t>
   </si>
 </sst>
 </file>
@@ -7758,7 +7800,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{29A1E198-E744-0F45-8483-AA87E5830D61}">
   <dimension ref="A1:B148"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A75" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F88" sqref="F88"/>
     </sheetView>
   </sheetViews>
@@ -8955,6 +8997,1254 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1D1E69E6-0320-4A4C-B581-483728603377}">
+  <dimension ref="A1:B153"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="44.83203125" customWidth="1"/>
+    <col min="2" max="2" width="33.1640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>44</v>
+      </c>
+      <c r="B2">
+        <v>392026.197319019</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>225</v>
+      </c>
+      <c r="B3">
+        <v>771983.32239999995</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>45</v>
+      </c>
+      <c r="B4">
+        <v>264152.43364930502</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>46</v>
+      </c>
+      <c r="B5">
+        <v>510287.181356752</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>160</v>
+      </c>
+      <c r="B6">
+        <v>1691150.70153317</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>161</v>
+      </c>
+      <c r="B7">
+        <v>448410.04944674397</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>167</v>
+      </c>
+      <c r="B8">
+        <v>2584874.9040020402</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>91</v>
+      </c>
+      <c r="B9">
+        <v>793333.33333333302</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>92</v>
+      </c>
+      <c r="B10">
+        <v>404644.32235354203</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>170</v>
+      </c>
+      <c r="B11">
+        <v>1691150.70153317</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>229</v>
+      </c>
+      <c r="B12">
+        <v>1139220.8972177</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>230</v>
+      </c>
+      <c r="B13">
+        <v>409626.53370758699</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>166</v>
+      </c>
+      <c r="B14">
+        <v>580607.882034485</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>29</v>
+      </c>
+      <c r="B15">
+        <v>2692574.9040020402</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>97</v>
+      </c>
+      <c r="B16">
+        <v>287417.48431020498</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>231</v>
+      </c>
+      <c r="B17">
+        <v>63333.333333333299</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>176</v>
+      </c>
+      <c r="B18">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>94</v>
+      </c>
+      <c r="B19">
+        <v>1314033.7881918801</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>95</v>
+      </c>
+      <c r="B20">
+        <v>766900.45252419403</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>35</v>
+      </c>
+      <c r="B21">
+        <v>25.920984480000001</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>47</v>
+      </c>
+      <c r="B22">
+        <v>5046.8439197540301</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>96</v>
+      </c>
+      <c r="B23">
+        <v>365365.4375</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>48</v>
+      </c>
+      <c r="B24">
+        <v>6437.1468134258603</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>51</v>
+      </c>
+      <c r="B25">
+        <v>195.75</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>98</v>
+      </c>
+      <c r="B26">
+        <v>575245.56851562799</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>52</v>
+      </c>
+      <c r="B27">
+        <v>1808.2629884031201</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
+        <v>53</v>
+      </c>
+      <c r="B28">
+        <v>13387.5</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
+        <v>54</v>
+      </c>
+      <c r="B29">
+        <v>9541.0832866056498</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
+        <v>215</v>
+      </c>
+      <c r="B30">
+        <v>5339511.8662871197</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A31" t="s">
+        <v>154</v>
+      </c>
+      <c r="B31">
+        <v>12901853.966758801</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A32" t="s">
+        <v>168</v>
+      </c>
+      <c r="B32">
+        <v>19420910.1530203</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A33" t="s">
+        <v>3</v>
+      </c>
+      <c r="B33">
+        <v>276268783.32202202</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A34" t="s">
+        <v>165</v>
+      </c>
+      <c r="B34">
+        <v>135592935.27812499</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A35" t="s">
+        <v>4</v>
+      </c>
+      <c r="B35">
+        <v>129225833.333333</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A36" t="s">
+        <v>159</v>
+      </c>
+      <c r="B36">
+        <v>5339511.8662871197</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A37" t="s">
+        <v>84</v>
+      </c>
+      <c r="B37">
+        <v>5504023.1669762796</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A38" t="s">
+        <v>85</v>
+      </c>
+      <c r="B38">
+        <v>8608640.9415249191</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A39" t="s">
+        <v>86</v>
+      </c>
+      <c r="B39">
+        <v>793333.33333333302</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A40" t="s">
+        <v>87</v>
+      </c>
+      <c r="B40">
+        <v>100225</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A41" t="s">
+        <v>88</v>
+      </c>
+      <c r="B41">
+        <v>6321027.9454843299</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A42" t="s">
+        <v>89</v>
+      </c>
+      <c r="B42">
+        <v>40000</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A43" t="s">
+        <v>90</v>
+      </c>
+      <c r="B43">
+        <v>9716387.6293499898</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A44" t="s">
+        <v>5</v>
+      </c>
+      <c r="B44">
+        <v>178999173.98829699</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A45" t="s">
+        <v>155</v>
+      </c>
+      <c r="B45">
+        <v>76566794.296346307</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A46" t="s">
+        <v>6</v>
+      </c>
+      <c r="B46">
+        <v>157393563.666666</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A47" t="s">
+        <v>156</v>
+      </c>
+      <c r="B47">
+        <v>180803216.39998901</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A48" t="s">
+        <v>37</v>
+      </c>
+      <c r="B48">
+        <v>34000</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A49" t="s">
+        <v>178</v>
+      </c>
+      <c r="B49">
+        <v>26320000</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A50" t="s">
+        <v>38</v>
+      </c>
+      <c r="B50">
+        <v>15969915.2575</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A51" t="s">
+        <v>138</v>
+      </c>
+      <c r="B51">
+        <v>47926596.969999999</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A52" t="s">
+        <v>39</v>
+      </c>
+      <c r="B52">
+        <v>51155234.429589003</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A53" t="s">
+        <v>40</v>
+      </c>
+      <c r="B53">
+        <v>3000000</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A54" t="s">
+        <v>124</v>
+      </c>
+      <c r="B54">
+        <v>1999.2794019999999</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A55" t="s">
+        <v>135</v>
+      </c>
+      <c r="B55">
+        <v>7789.1925490000003</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A56" t="s">
+        <v>136</v>
+      </c>
+      <c r="B56">
+        <v>86884.467919999996</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A57" t="s">
+        <v>24</v>
+      </c>
+      <c r="B57">
+        <v>389718771.83409399</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A58" t="s">
+        <v>25</v>
+      </c>
+      <c r="B58">
+        <v>552526594.77124095</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A59" t="s">
+        <v>41</v>
+      </c>
+      <c r="B59">
+        <v>15172516.666666601</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A60" t="s">
+        <v>42</v>
+      </c>
+      <c r="B60">
+        <v>1459010</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A61" t="s">
+        <v>7</v>
+      </c>
+      <c r="B61">
+        <v>264584522.65961</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A62" t="s">
+        <v>43</v>
+      </c>
+      <c r="B62">
+        <v>27600432.865182701</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A63" t="s">
+        <v>125</v>
+      </c>
+      <c r="B63">
+        <v>1999.2794019999999</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A64" t="s">
+        <v>137</v>
+      </c>
+      <c r="B64">
+        <v>321203.81650000002</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A65" t="s">
+        <v>224</v>
+      </c>
+      <c r="B65">
+        <v>6634766.74125</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A66" t="s">
+        <v>22</v>
+      </c>
+      <c r="B66">
+        <v>6634766.74125</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A67" t="s">
+        <v>8</v>
+      </c>
+      <c r="B67">
+        <v>137557916.73517799</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A68" t="s">
+        <v>9</v>
+      </c>
+      <c r="B68">
+        <v>253870375.16864401</v>
+      </c>
+    </row>
+    <row r="69" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A69" t="s">
+        <v>164</v>
+      </c>
+      <c r="B69">
+        <v>133533353.718908</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A70" t="s">
+        <v>14</v>
+      </c>
+      <c r="B70">
+        <v>49359622.369231403</v>
+      </c>
+    </row>
+    <row r="71" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A71" t="s">
+        <v>10</v>
+      </c>
+      <c r="B71">
+        <v>112037800</v>
+      </c>
+    </row>
+    <row r="72" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A72" t="s">
+        <v>157</v>
+      </c>
+      <c r="B72">
+        <v>29085600</v>
+      </c>
+    </row>
+    <row r="73" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A73" t="s">
+        <v>11</v>
+      </c>
+      <c r="B73">
+        <v>240498185.091364</v>
+      </c>
+    </row>
+    <row r="74" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A74" t="s">
+        <v>26</v>
+      </c>
+      <c r="B74">
+        <v>531768.44999999995</v>
+      </c>
+    </row>
+    <row r="75" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A75" t="s">
+        <v>27</v>
+      </c>
+      <c r="B75">
+        <v>531768.44999999995</v>
+      </c>
+    </row>
+    <row r="76" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A76" t="s">
+        <v>28</v>
+      </c>
+      <c r="B76">
+        <v>1643536.0106001699</v>
+      </c>
+    </row>
+    <row r="77" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A77" t="s">
+        <v>228</v>
+      </c>
+      <c r="B77">
+        <v>1139220.8972177</v>
+      </c>
+    </row>
+    <row r="78" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A78" t="s">
+        <v>226</v>
+      </c>
+      <c r="B78">
+        <v>409626.53370758699</v>
+      </c>
+    </row>
+    <row r="79" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A79" t="s">
+        <v>171</v>
+      </c>
+      <c r="B79">
+        <v>1691150.70153317</v>
+      </c>
+    </row>
+    <row r="80" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A80" t="s">
+        <v>109</v>
+      </c>
+      <c r="B80">
+        <v>580607.882034485</v>
+      </c>
+    </row>
+    <row r="81" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A81" t="s">
+        <v>30</v>
+      </c>
+      <c r="B81">
+        <v>2692574.9040020402</v>
+      </c>
+    </row>
+    <row r="82" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A82" t="s">
+        <v>105</v>
+      </c>
+      <c r="B82">
+        <v>287417.48431020498</v>
+      </c>
+    </row>
+    <row r="83" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A83" t="s">
+        <v>227</v>
+      </c>
+      <c r="B83">
+        <v>63333.333333333299</v>
+      </c>
+    </row>
+    <row r="84" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A84" t="s">
+        <v>99</v>
+      </c>
+      <c r="B84">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="85" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A85" t="s">
+        <v>100</v>
+      </c>
+      <c r="B85">
+        <v>923.33333333333303</v>
+      </c>
+    </row>
+    <row r="86" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A86" t="s">
+        <v>101</v>
+      </c>
+      <c r="B86">
+        <v>1226.6666666666599</v>
+      </c>
+    </row>
+    <row r="87" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A87" t="s">
+        <v>185</v>
+      </c>
+      <c r="B87">
+        <v>21.588666666666601</v>
+      </c>
+    </row>
+    <row r="88" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A88" t="s">
+        <v>36</v>
+      </c>
+      <c r="B88">
+        <v>25.920864000000002</v>
+      </c>
+    </row>
+    <row r="89" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A89" t="s">
+        <v>55</v>
+      </c>
+      <c r="B89">
+        <v>351.612451979838</v>
+      </c>
+    </row>
+    <row r="90" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A90" t="s">
+        <v>56</v>
+      </c>
+      <c r="B90">
+        <v>400.12225003956598</v>
+      </c>
+    </row>
+    <row r="91" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A91" t="s">
+        <v>57</v>
+      </c>
+      <c r="B91">
+        <v>542.34540101064101</v>
+      </c>
+    </row>
+    <row r="92" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A92" t="s">
+        <v>59</v>
+      </c>
+      <c r="B92">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="93" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A93" t="s">
+        <v>102</v>
+      </c>
+      <c r="B93">
+        <v>1031.35466666666</v>
+      </c>
+    </row>
+    <row r="94" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A94" t="s">
+        <v>103</v>
+      </c>
+      <c r="B94">
+        <v>1334.6880000000001</v>
+      </c>
+    </row>
+    <row r="95" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A95" t="s">
+        <v>217</v>
+      </c>
+      <c r="B95">
+        <v>664.02036322137997</v>
+      </c>
+    </row>
+    <row r="96" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A96" t="s">
+        <v>108</v>
+      </c>
+      <c r="B96">
+        <v>933.33333333333303</v>
+      </c>
+    </row>
+    <row r="97" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A97" t="s">
+        <v>60</v>
+      </c>
+      <c r="B97">
+        <v>427.23471765693802</v>
+      </c>
+    </row>
+    <row r="98" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A98" t="s">
+        <v>61</v>
+      </c>
+      <c r="B98">
+        <v>752.12698196337703</v>
+      </c>
+    </row>
+    <row r="99" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A99" t="s">
+        <v>63</v>
+      </c>
+      <c r="B99">
+        <v>262.88240028896502</v>
+      </c>
+    </row>
+    <row r="100" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A100" t="s">
+        <v>17</v>
+      </c>
+      <c r="B100">
+        <v>2453.3333333333298</v>
+      </c>
+    </row>
+    <row r="101" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A101" t="s">
+        <v>106</v>
+      </c>
+      <c r="B101">
+        <v>1053.3306250000001</v>
+      </c>
+    </row>
+    <row r="102" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A102" t="s">
+        <v>107</v>
+      </c>
+      <c r="B102">
+        <v>1356.62929166666</v>
+      </c>
+    </row>
+    <row r="103" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A103" t="s">
+        <v>216</v>
+      </c>
+      <c r="B103">
+        <v>679.91573362229894</v>
+      </c>
+    </row>
+    <row r="104" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A104" t="s">
+        <v>110</v>
+      </c>
+      <c r="B104">
+        <v>933.33333333333303</v>
+      </c>
+    </row>
+    <row r="105" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A105" t="s">
+        <v>67</v>
+      </c>
+      <c r="B105">
+        <v>118.803622278709</v>
+      </c>
+    </row>
+    <row r="106" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A106" t="s">
+        <v>68</v>
+      </c>
+      <c r="B106">
+        <v>14.7</v>
+      </c>
+    </row>
+    <row r="107" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A107" t="s">
+        <v>69</v>
+      </c>
+      <c r="B107">
+        <v>95.55</v>
+      </c>
+    </row>
+    <row r="108" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A108" t="s">
+        <v>173</v>
+      </c>
+      <c r="B108">
+        <v>5339511.8662871197</v>
+      </c>
+    </row>
+    <row r="109" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A109" t="s">
+        <v>209</v>
+      </c>
+      <c r="B109">
+        <v>5197731.9613897596</v>
+      </c>
+    </row>
+    <row r="110" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A110" t="s">
+        <v>211</v>
+      </c>
+      <c r="B110">
+        <v>7573760.8167445101</v>
+      </c>
+    </row>
+    <row r="111" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A111" t="s">
+        <v>235</v>
+      </c>
+      <c r="B111">
+        <v>15439666.448000001</v>
+      </c>
+    </row>
+    <row r="112" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A112" t="s">
+        <v>208</v>
+      </c>
+      <c r="B112">
+        <v>5339511.8662871197</v>
+      </c>
+    </row>
+    <row r="113" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A113" t="s">
+        <v>210</v>
+      </c>
+      <c r="B113">
+        <v>9825516.7771235704</v>
+      </c>
+    </row>
+    <row r="114" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A114" t="s">
+        <v>194</v>
+      </c>
+      <c r="B114">
+        <v>5197731.9613897596</v>
+      </c>
+    </row>
+    <row r="115" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A115" t="s">
+        <v>196</v>
+      </c>
+      <c r="B115">
+        <v>7573760.8167445101</v>
+      </c>
+    </row>
+    <row r="116" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A116" t="s">
+        <v>236</v>
+      </c>
+      <c r="B116">
+        <v>15439666.448000001</v>
+      </c>
+    </row>
+    <row r="117" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A117" t="s">
+        <v>213</v>
+      </c>
+      <c r="B117">
+        <v>5339511.8662871197</v>
+      </c>
+    </row>
+    <row r="118" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A118" t="s">
+        <v>212</v>
+      </c>
+      <c r="B118">
+        <v>9825516.7771235704</v>
+      </c>
+    </row>
+    <row r="119" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A119" t="s">
+        <v>186</v>
+      </c>
+      <c r="B119">
+        <v>400000</v>
+      </c>
+    </row>
+    <row r="120" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A120" t="s">
+        <v>193</v>
+      </c>
+      <c r="B120">
+        <v>454750</v>
+      </c>
+    </row>
+    <row r="121" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A121" t="s">
+        <v>195</v>
+      </c>
+      <c r="B121">
+        <v>173333.33333333299</v>
+      </c>
+    </row>
+    <row r="122" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A122" t="s">
+        <v>192</v>
+      </c>
+      <c r="B122">
+        <v>893566.66666666605</v>
+      </c>
+    </row>
+    <row r="123" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A123" t="s">
+        <v>199</v>
+      </c>
+      <c r="B123">
+        <v>5197731.9613897596</v>
+      </c>
+    </row>
+    <row r="124" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A124" t="s">
+        <v>198</v>
+      </c>
+      <c r="B124">
+        <v>7573760.8167445101</v>
+      </c>
+    </row>
+    <row r="125" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A125" t="s">
+        <v>232</v>
+      </c>
+      <c r="B125">
+        <v>15439666.448000001</v>
+      </c>
+    </row>
+    <row r="126" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A126" t="s">
+        <v>197</v>
+      </c>
+      <c r="B126">
+        <v>5339511.8662871197</v>
+      </c>
+    </row>
+    <row r="127" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A127" t="s">
+        <v>200</v>
+      </c>
+      <c r="B127">
+        <v>9825516.7771235704</v>
+      </c>
+    </row>
+    <row r="128" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A128" t="s">
+        <v>187</v>
+      </c>
+      <c r="B128">
+        <v>400000</v>
+      </c>
+    </row>
+    <row r="129" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A129" t="s">
+        <v>12</v>
+      </c>
+      <c r="B129">
+        <v>19071729.917292699</v>
+      </c>
+    </row>
+    <row r="130" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A130" t="s">
+        <v>162</v>
+      </c>
+      <c r="B130">
+        <v>142751.984952906</v>
+      </c>
+    </row>
+    <row r="131" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A131" t="s">
+        <v>163</v>
+      </c>
+      <c r="B131">
+        <v>12364158.3124649</v>
+      </c>
+    </row>
+    <row r="132" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A132" t="s">
+        <v>2</v>
+      </c>
+      <c r="B132">
+        <v>5300353.2122133197</v>
+      </c>
+    </row>
+    <row r="133" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A133" t="s">
+        <v>201</v>
+      </c>
+      <c r="B133">
+        <v>5197731.9613897596</v>
+      </c>
+    </row>
+    <row r="134" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A134" t="s">
+        <v>191</v>
+      </c>
+      <c r="B134">
+        <v>7573760.8167445101</v>
+      </c>
+    </row>
+    <row r="135" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A135" t="s">
+        <v>234</v>
+      </c>
+      <c r="B135">
+        <v>15439666.448000001</v>
+      </c>
+    </row>
+    <row r="136" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A136" t="s">
+        <v>190</v>
+      </c>
+      <c r="B136">
+        <v>5339511.8662871197</v>
+      </c>
+    </row>
+    <row r="137" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A137" t="s">
+        <v>189</v>
+      </c>
+      <c r="B137">
+        <v>9825516.7771235704</v>
+      </c>
+    </row>
+    <row r="138" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A138" t="s">
+        <v>188</v>
+      </c>
+      <c r="B138">
+        <v>400000</v>
+      </c>
+    </row>
+    <row r="139" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A139" t="s">
+        <v>214</v>
+      </c>
+      <c r="B139">
+        <v>454750</v>
+      </c>
+    </row>
+    <row r="140" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A140" t="s">
+        <v>175</v>
+      </c>
+      <c r="B140">
+        <v>4211732.8228744604</v>
+      </c>
+    </row>
+    <row r="141" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A141" t="s">
+        <v>207</v>
+      </c>
+      <c r="B141">
+        <v>5197731.9613897596</v>
+      </c>
+    </row>
+    <row r="142" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A142" t="s">
+        <v>203</v>
+      </c>
+      <c r="B142">
+        <v>7573760.8167445101</v>
+      </c>
+    </row>
+    <row r="143" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A143" t="s">
+        <v>233</v>
+      </c>
+      <c r="B143">
+        <v>15439666.448000001</v>
+      </c>
+    </row>
+    <row r="144" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A144" t="s">
+        <v>206</v>
+      </c>
+      <c r="B144">
+        <v>5339511.8662871197</v>
+      </c>
+    </row>
+    <row r="145" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A145" t="s">
+        <v>204</v>
+      </c>
+      <c r="B145">
+        <v>9825516.7771235704</v>
+      </c>
+    </row>
+    <row r="146" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A146" t="s">
+        <v>202</v>
+      </c>
+      <c r="B146">
+        <v>400000</v>
+      </c>
+    </row>
+    <row r="147" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A147" t="s">
+        <v>205</v>
+      </c>
+      <c r="B147">
+        <v>454750</v>
+      </c>
+    </row>
+    <row r="148" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A148" t="s">
+        <v>174</v>
+      </c>
+      <c r="B148">
+        <v>3777132.2356575001</v>
+      </c>
+    </row>
+    <row r="149" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A149" t="s">
+        <v>172</v>
+      </c>
+      <c r="B149">
+        <v>5339511.8662871197</v>
+      </c>
+    </row>
+    <row r="150" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A150" t="s">
+        <v>79</v>
+      </c>
+      <c r="B150">
+        <v>5197731.9613897596</v>
+      </c>
+    </row>
+    <row r="151" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A151" t="s">
+        <v>80</v>
+      </c>
+      <c r="B151">
+        <v>392026.197319019</v>
+      </c>
+    </row>
+    <row r="152" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A152" t="s">
+        <v>81</v>
+      </c>
+      <c r="B152">
+        <v>264152.43364930502</v>
+      </c>
+    </row>
+    <row r="153" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A153" t="s">
+        <v>82</v>
+      </c>
+      <c r="B153">
+        <v>510287.181356752</v>
+      </c>
+    </row>
+  </sheetData>
+  <autoFilter ref="A1:B153" xr:uid="{55F4835A-4B06-5640-97B8-B7039B4C53F4}">
+    <sortState ref="A2:B153">
+      <sortCondition ref="A1:A153"/>
+    </sortState>
+  </autoFilter>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Changed the costs, which were affected by the changed merit order, due to imported electricity
</commit_message>
<xml_diff>
--- a/scripts/query_generator/cost_update/cost_inputs.xlsx
+++ b/scripts/query_generator/cost_update/cost_inputs.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10523"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10116"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/marliekeverweij/Projects/mechanical_turk/scripts/query_generator/cost_update/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/martlubben/Projects/mechanical_turk/scripts/query_generator/cost_update/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B6DEE0F-4890-AB49-A29A-46962449989A}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="26800" tabRatio="500" firstSheet="3" activeTab="15" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="440" windowWidth="25600" windowHeight="17480" tabRatio="500" firstSheet="4" activeTab="16" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="20131125" sheetId="7" r:id="rId1"/>
@@ -29,6 +28,7 @@
     <sheet name="20180103" sheetId="14" r:id="rId14"/>
     <sheet name="20180302" sheetId="15" r:id="rId15"/>
     <sheet name="20180612" sheetId="16" r:id="rId16"/>
+    <sheet name="20180628" sheetId="17" r:id="rId17"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">'20121221'!$A$1:$B$116</definedName>
@@ -56,7 +56,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2119" uniqueCount="237">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2275" uniqueCount="237">
   <si>
     <t>key</t>
   </si>
@@ -9004,7 +9004,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1D1E69E6-0320-4A4C-B581-483728603377}">
   <dimension ref="A1:B153"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
@@ -10244,6 +10244,1268 @@
       <sortCondition ref="A1:A153"/>
     </sortState>
   </autoFilter>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FE698956-C4B7-4545-BA93-E6CA6D592972}">
+  <dimension ref="A1:B155"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E17" sqref="E17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="44.5" customWidth="1"/>
+    <col min="2" max="2" width="36.5" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>44</v>
+      </c>
+      <c r="B2">
+        <v>392026.197319019</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>225</v>
+      </c>
+      <c r="B3">
+        <v>771983.32239999995</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>45</v>
+      </c>
+      <c r="B4">
+        <v>264152.43364930502</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>46</v>
+      </c>
+      <c r="B5">
+        <v>510287.181356752</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>160</v>
+      </c>
+      <c r="B6">
+        <v>1691150.70153317</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>161</v>
+      </c>
+      <c r="B7">
+        <v>448410.04944674397</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>167</v>
+      </c>
+      <c r="B8">
+        <v>2584874.9040020402</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>91</v>
+      </c>
+      <c r="B9">
+        <v>793333.33333333302</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>92</v>
+      </c>
+      <c r="B10">
+        <v>404644.32235354203</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>170</v>
+      </c>
+      <c r="B11">
+        <v>1691150.70153317</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>229</v>
+      </c>
+      <c r="B12">
+        <v>1139220.8972177</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>230</v>
+      </c>
+      <c r="B13">
+        <v>409626.53370758699</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>166</v>
+      </c>
+      <c r="B14">
+        <v>580607.882034485</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>29</v>
+      </c>
+      <c r="B15">
+        <v>2692574.9040020402</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>97</v>
+      </c>
+      <c r="B16">
+        <v>287417.48431020498</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>231</v>
+      </c>
+      <c r="B17">
+        <v>63333.333333333299</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>176</v>
+      </c>
+      <c r="B18">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>94</v>
+      </c>
+      <c r="B19">
+        <v>1314033.7881918801</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>95</v>
+      </c>
+      <c r="B20">
+        <v>766900.45252419403</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>35</v>
+      </c>
+      <c r="B21">
+        <v>25.920984480000001</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>47</v>
+      </c>
+      <c r="B22">
+        <v>5046.8439197540301</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>96</v>
+      </c>
+      <c r="B23">
+        <v>365365.4375</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>48</v>
+      </c>
+      <c r="B24">
+        <v>6437.1468134258603</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>51</v>
+      </c>
+      <c r="B25">
+        <v>195.75</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>98</v>
+      </c>
+      <c r="B26">
+        <v>575245.56851562799</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>52</v>
+      </c>
+      <c r="B27">
+        <v>1808.2629884031201</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
+        <v>53</v>
+      </c>
+      <c r="B28">
+        <v>13387.5</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
+        <v>54</v>
+      </c>
+      <c r="B29">
+        <v>9541.0832866056498</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
+        <v>215</v>
+      </c>
+      <c r="B30">
+        <v>5339511.8662871197</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A31" t="s">
+        <v>154</v>
+      </c>
+      <c r="B31">
+        <v>12381000</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A32" t="s">
+        <v>168</v>
+      </c>
+      <c r="B32">
+        <v>19420910.1530203</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A33" t="s">
+        <v>3</v>
+      </c>
+      <c r="B33">
+        <v>276268783.32202202</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A34" t="s">
+        <v>165</v>
+      </c>
+      <c r="B34">
+        <v>135592935.27812499</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A35" t="s">
+        <v>4</v>
+      </c>
+      <c r="B35">
+        <v>129225833.333333</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A36" t="s">
+        <v>159</v>
+      </c>
+      <c r="B36">
+        <v>5339511.8662871197</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A37" t="s">
+        <v>84</v>
+      </c>
+      <c r="B37">
+        <v>5504023.1669762796</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A38" t="s">
+        <v>85</v>
+      </c>
+      <c r="B38">
+        <v>8608640.9415249191</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A39" t="s">
+        <v>86</v>
+      </c>
+      <c r="B39">
+        <v>793333.33333333302</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A40" t="s">
+        <v>87</v>
+      </c>
+      <c r="B40">
+        <v>100225</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A41" t="s">
+        <v>88</v>
+      </c>
+      <c r="B41">
+        <v>6321027.9454843299</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A42" t="s">
+        <v>89</v>
+      </c>
+      <c r="B42">
+        <v>40000</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A43" t="s">
+        <v>90</v>
+      </c>
+      <c r="B43">
+        <v>9716387.6293499898</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A44" t="s">
+        <v>5</v>
+      </c>
+      <c r="B44">
+        <v>178999173.98829699</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A45" t="s">
+        <v>155</v>
+      </c>
+      <c r="B45">
+        <v>76566794.296346307</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A46" t="s">
+        <v>6</v>
+      </c>
+      <c r="B46">
+        <v>157393563.666666</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A47" t="s">
+        <v>156</v>
+      </c>
+      <c r="B47">
+        <v>180803216.39998901</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A48" t="s">
+        <v>37</v>
+      </c>
+      <c r="B48">
+        <v>34000</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A49" t="s">
+        <v>178</v>
+      </c>
+      <c r="B49">
+        <v>26320000</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A50" t="s">
+        <v>38</v>
+      </c>
+      <c r="B50">
+        <v>15969915.2575</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A51" t="s">
+        <v>138</v>
+      </c>
+      <c r="B51">
+        <v>47926596.969999999</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A52" t="s">
+        <v>39</v>
+      </c>
+      <c r="B52">
+        <v>51155234.429589003</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A53" t="s">
+        <v>40</v>
+      </c>
+      <c r="B53">
+        <v>3000000</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A54" t="s">
+        <v>124</v>
+      </c>
+      <c r="B54">
+        <v>1999.2794019999999</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A55" t="s">
+        <v>135</v>
+      </c>
+      <c r="B55">
+        <v>7789.1925490000003</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A56" t="s">
+        <v>136</v>
+      </c>
+      <c r="B56">
+        <v>86884.467919999996</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A57" t="s">
+        <v>24</v>
+      </c>
+      <c r="B57">
+        <v>389718771.83409399</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A58" t="s">
+        <v>25</v>
+      </c>
+      <c r="B58">
+        <v>552526594.77124095</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A59" t="s">
+        <v>41</v>
+      </c>
+      <c r="B59">
+        <v>15172516.666666601</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A60" t="s">
+        <v>42</v>
+      </c>
+      <c r="B60">
+        <v>1459010</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A61" t="s">
+        <v>7</v>
+      </c>
+      <c r="B61">
+        <v>264584522.65961</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A62" t="s">
+        <v>43</v>
+      </c>
+      <c r="B62">
+        <v>27600432.865182701</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A63" t="s">
+        <v>125</v>
+      </c>
+      <c r="B63">
+        <v>1999.2794019999999</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A64" t="s">
+        <v>137</v>
+      </c>
+      <c r="B64">
+        <v>321203.81650000002</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A65" t="s">
+        <v>224</v>
+      </c>
+      <c r="B65">
+        <v>6634766.74125</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A66" t="s">
+        <v>22</v>
+      </c>
+      <c r="B66">
+        <v>6634766.74125</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A67" t="s">
+        <v>8</v>
+      </c>
+      <c r="B67">
+        <v>137557916.73517799</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A68" t="s">
+        <v>9</v>
+      </c>
+      <c r="B68">
+        <v>253870375.16864401</v>
+      </c>
+    </row>
+    <row r="69" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A69" t="s">
+        <v>164</v>
+      </c>
+      <c r="B69">
+        <v>117461956.55625001</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A70" t="s">
+        <v>14</v>
+      </c>
+      <c r="B70">
+        <v>49359622.369231403</v>
+      </c>
+    </row>
+    <row r="71" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A71" t="s">
+        <v>10</v>
+      </c>
+      <c r="B71">
+        <v>112037800</v>
+      </c>
+    </row>
+    <row r="72" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A72" t="s">
+        <v>157</v>
+      </c>
+      <c r="B72">
+        <v>29085600</v>
+      </c>
+    </row>
+    <row r="73" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A73" t="s">
+        <v>11</v>
+      </c>
+      <c r="B73">
+        <v>240498185.091364</v>
+      </c>
+    </row>
+    <row r="74" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A74" t="s">
+        <v>26</v>
+      </c>
+      <c r="B74">
+        <v>531768.44999999995</v>
+      </c>
+    </row>
+    <row r="75" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A75" t="s">
+        <v>27</v>
+      </c>
+      <c r="B75">
+        <v>531768.44999999995</v>
+      </c>
+    </row>
+    <row r="76" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A76" t="s">
+        <v>28</v>
+      </c>
+      <c r="B76">
+        <v>1643536.0106001699</v>
+      </c>
+    </row>
+    <row r="77" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A77" t="s">
+        <v>228</v>
+      </c>
+      <c r="B77">
+        <v>1139220.8972177</v>
+      </c>
+    </row>
+    <row r="78" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A78" t="s">
+        <v>226</v>
+      </c>
+      <c r="B78">
+        <v>409626.53370758699</v>
+      </c>
+    </row>
+    <row r="79" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A79" t="s">
+        <v>171</v>
+      </c>
+      <c r="B79">
+        <v>1691150.70153317</v>
+      </c>
+    </row>
+    <row r="80" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A80" t="s">
+        <v>109</v>
+      </c>
+      <c r="B80">
+        <v>580607.882034485</v>
+      </c>
+    </row>
+    <row r="81" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A81" t="s">
+        <v>30</v>
+      </c>
+      <c r="B81">
+        <v>2692574.9040020402</v>
+      </c>
+    </row>
+    <row r="82" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A82" t="s">
+        <v>105</v>
+      </c>
+      <c r="B82">
+        <v>287417.48431020498</v>
+      </c>
+    </row>
+    <row r="83" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A83" t="s">
+        <v>227</v>
+      </c>
+      <c r="B83">
+        <v>63333.333333333299</v>
+      </c>
+    </row>
+    <row r="84" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A84" t="s">
+        <v>99</v>
+      </c>
+      <c r="B84">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="85" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A85" t="s">
+        <v>100</v>
+      </c>
+      <c r="B85">
+        <v>923.33333333333303</v>
+      </c>
+    </row>
+    <row r="86" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A86" t="s">
+        <v>101</v>
+      </c>
+      <c r="B86">
+        <v>1226.6666666666599</v>
+      </c>
+    </row>
+    <row r="87" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A87" t="s">
+        <v>185</v>
+      </c>
+      <c r="B87">
+        <v>21.588666666666601</v>
+      </c>
+    </row>
+    <row r="88" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A88" t="s">
+        <v>36</v>
+      </c>
+      <c r="B88">
+        <v>25.920864000000002</v>
+      </c>
+    </row>
+    <row r="89" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A89" t="s">
+        <v>55</v>
+      </c>
+      <c r="B89">
+        <v>351.612451979838</v>
+      </c>
+    </row>
+    <row r="90" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A90" t="s">
+        <v>56</v>
+      </c>
+      <c r="B90">
+        <v>400.12225003956598</v>
+      </c>
+    </row>
+    <row r="91" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A91" t="s">
+        <v>57</v>
+      </c>
+      <c r="B91">
+        <v>542.34540101064101</v>
+      </c>
+    </row>
+    <row r="92" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A92" t="s">
+        <v>59</v>
+      </c>
+      <c r="B92">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="93" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A93" t="s">
+        <v>102</v>
+      </c>
+      <c r="B93">
+        <v>1031.35466666666</v>
+      </c>
+    </row>
+    <row r="94" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A94" t="s">
+        <v>103</v>
+      </c>
+      <c r="B94">
+        <v>1334.6880000000001</v>
+      </c>
+    </row>
+    <row r="95" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A95" t="s">
+        <v>217</v>
+      </c>
+      <c r="B95">
+        <v>664.02036322137997</v>
+      </c>
+    </row>
+    <row r="96" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A96" t="s">
+        <v>108</v>
+      </c>
+      <c r="B96">
+        <v>933.33333333333303</v>
+      </c>
+    </row>
+    <row r="97" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A97" t="s">
+        <v>60</v>
+      </c>
+      <c r="B97">
+        <v>427.23471765693802</v>
+      </c>
+    </row>
+    <row r="98" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A98" t="s">
+        <v>61</v>
+      </c>
+      <c r="B98">
+        <v>752.12698196337703</v>
+      </c>
+    </row>
+    <row r="99" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A99" t="s">
+        <v>63</v>
+      </c>
+      <c r="B99">
+        <v>262.88240028896502</v>
+      </c>
+    </row>
+    <row r="100" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A100" t="s">
+        <v>17</v>
+      </c>
+      <c r="B100">
+        <v>2453.3333333333298</v>
+      </c>
+    </row>
+    <row r="101" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A101" t="s">
+        <v>106</v>
+      </c>
+      <c r="B101">
+        <v>1053.3306250000001</v>
+      </c>
+    </row>
+    <row r="102" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A102" t="s">
+        <v>107</v>
+      </c>
+      <c r="B102">
+        <v>1356.62929166666</v>
+      </c>
+    </row>
+    <row r="103" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A103" t="s">
+        <v>216</v>
+      </c>
+      <c r="B103">
+        <v>679.91573362229894</v>
+      </c>
+    </row>
+    <row r="104" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A104" t="s">
+        <v>110</v>
+      </c>
+      <c r="B104">
+        <v>933.33333333333303</v>
+      </c>
+    </row>
+    <row r="105" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A105" t="s">
+        <v>67</v>
+      </c>
+      <c r="B105">
+        <v>118.803622278709</v>
+      </c>
+    </row>
+    <row r="106" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A106" t="s">
+        <v>68</v>
+      </c>
+      <c r="B106">
+        <v>14.7</v>
+      </c>
+    </row>
+    <row r="107" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A107" t="s">
+        <v>69</v>
+      </c>
+      <c r="B107">
+        <v>95.55</v>
+      </c>
+    </row>
+    <row r="108" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A108" t="s">
+        <v>173</v>
+      </c>
+      <c r="B108">
+        <v>5339511.8662871197</v>
+      </c>
+    </row>
+    <row r="109" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A109" t="s">
+        <v>209</v>
+      </c>
+      <c r="B109">
+        <v>5197731.9613897596</v>
+      </c>
+    </row>
+    <row r="110" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A110" t="s">
+        <v>211</v>
+      </c>
+      <c r="B110">
+        <v>7573760.8167445101</v>
+      </c>
+    </row>
+    <row r="111" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A111" t="s">
+        <v>235</v>
+      </c>
+      <c r="B111">
+        <v>15439666.448000001</v>
+      </c>
+    </row>
+    <row r="112" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A112" t="s">
+        <v>208</v>
+      </c>
+      <c r="B112">
+        <v>5339511.8662871197</v>
+      </c>
+    </row>
+    <row r="113" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A113" t="s">
+        <v>210</v>
+      </c>
+      <c r="B113">
+        <v>9825516.7771235704</v>
+      </c>
+    </row>
+    <row r="114" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A114" t="s">
+        <v>194</v>
+      </c>
+      <c r="B114">
+        <v>5197731.9613897596</v>
+      </c>
+    </row>
+    <row r="115" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A115" t="s">
+        <v>196</v>
+      </c>
+      <c r="B115">
+        <v>7573760.8167445101</v>
+      </c>
+    </row>
+    <row r="116" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A116" t="s">
+        <v>236</v>
+      </c>
+      <c r="B116">
+        <v>15439666.448000001</v>
+      </c>
+    </row>
+    <row r="117" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A117" t="s">
+        <v>213</v>
+      </c>
+      <c r="B117">
+        <v>5339511.8662871197</v>
+      </c>
+    </row>
+    <row r="118" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A118" t="s">
+        <v>212</v>
+      </c>
+      <c r="B118">
+        <v>9825516.7771235704</v>
+      </c>
+    </row>
+    <row r="119" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A119" t="s">
+        <v>186</v>
+      </c>
+      <c r="B119">
+        <v>400000</v>
+      </c>
+    </row>
+    <row r="120" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A120" t="s">
+        <v>193</v>
+      </c>
+      <c r="B120">
+        <v>454750</v>
+      </c>
+    </row>
+    <row r="121" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A121" t="s">
+        <v>195</v>
+      </c>
+      <c r="B121">
+        <v>173333.33333333299</v>
+      </c>
+    </row>
+    <row r="122" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A122" t="s">
+        <v>192</v>
+      </c>
+      <c r="B122">
+        <v>893566.66666666605</v>
+      </c>
+    </row>
+    <row r="123" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A123" t="s">
+        <v>199</v>
+      </c>
+      <c r="B123">
+        <v>5197731.9613897596</v>
+      </c>
+    </row>
+    <row r="124" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A124" t="s">
+        <v>198</v>
+      </c>
+      <c r="B124">
+        <v>7573760.8167445101</v>
+      </c>
+    </row>
+    <row r="125" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A125" t="s">
+        <v>232</v>
+      </c>
+      <c r="B125">
+        <v>15439666.448000001</v>
+      </c>
+    </row>
+    <row r="126" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A126" t="s">
+        <v>197</v>
+      </c>
+      <c r="B126">
+        <v>5339511.8662871197</v>
+      </c>
+    </row>
+    <row r="127" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A127" t="s">
+        <v>200</v>
+      </c>
+      <c r="B127">
+        <v>9825516.7771235704</v>
+      </c>
+    </row>
+    <row r="128" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A128" t="s">
+        <v>187</v>
+      </c>
+      <c r="B128">
+        <v>400000</v>
+      </c>
+    </row>
+    <row r="129" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A129" t="s">
+        <v>12</v>
+      </c>
+      <c r="B129">
+        <v>19071729.917292699</v>
+      </c>
+    </row>
+    <row r="130" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A130" t="s">
+        <v>162</v>
+      </c>
+      <c r="B130">
+        <v>142751.984952906</v>
+      </c>
+    </row>
+    <row r="131" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A131" t="s">
+        <v>163</v>
+      </c>
+      <c r="B131">
+        <v>12364158.3124649</v>
+      </c>
+    </row>
+    <row r="132" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A132" t="s">
+        <v>2</v>
+      </c>
+      <c r="B132">
+        <v>5300353.2122133197</v>
+      </c>
+    </row>
+    <row r="133" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A133" t="s">
+        <v>201</v>
+      </c>
+      <c r="B133">
+        <v>5197731.9613897596</v>
+      </c>
+    </row>
+    <row r="134" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A134" t="s">
+        <v>191</v>
+      </c>
+      <c r="B134">
+        <v>7573760.8167445101</v>
+      </c>
+    </row>
+    <row r="135" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A135" t="s">
+        <v>234</v>
+      </c>
+      <c r="B135">
+        <v>15439666.448000001</v>
+      </c>
+    </row>
+    <row r="136" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A136" t="s">
+        <v>190</v>
+      </c>
+      <c r="B136">
+        <v>5339511.8662871197</v>
+      </c>
+    </row>
+    <row r="137" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A137" t="s">
+        <v>189</v>
+      </c>
+      <c r="B137">
+        <v>9825516.7771235704</v>
+      </c>
+    </row>
+    <row r="138" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A138" t="s">
+        <v>188</v>
+      </c>
+      <c r="B138">
+        <v>400000</v>
+      </c>
+    </row>
+    <row r="139" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A139" t="s">
+        <v>214</v>
+      </c>
+      <c r="B139">
+        <v>454750</v>
+      </c>
+    </row>
+    <row r="140" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A140" t="s">
+        <v>175</v>
+      </c>
+      <c r="B140">
+        <v>4211732.8228744604</v>
+      </c>
+    </row>
+    <row r="141" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A141" t="s">
+        <v>207</v>
+      </c>
+      <c r="B141">
+        <v>5197731.9613897596</v>
+      </c>
+    </row>
+    <row r="142" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A142" t="s">
+        <v>203</v>
+      </c>
+      <c r="B142">
+        <v>7573760.8167445101</v>
+      </c>
+    </row>
+    <row r="143" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A143" t="s">
+        <v>233</v>
+      </c>
+      <c r="B143">
+        <v>15439666.448000001</v>
+      </c>
+    </row>
+    <row r="144" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A144" t="s">
+        <v>206</v>
+      </c>
+      <c r="B144">
+        <v>5339511.8662871197</v>
+      </c>
+    </row>
+    <row r="145" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A145" t="s">
+        <v>204</v>
+      </c>
+      <c r="B145">
+        <v>9825516.7771235704</v>
+      </c>
+    </row>
+    <row r="146" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A146" t="s">
+        <v>202</v>
+      </c>
+      <c r="B146">
+        <v>400000</v>
+      </c>
+    </row>
+    <row r="147" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A147" t="s">
+        <v>205</v>
+      </c>
+      <c r="B147">
+        <v>454750</v>
+      </c>
+    </row>
+    <row r="148" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A148" t="s">
+        <v>174</v>
+      </c>
+      <c r="B148">
+        <v>3777132.2356575001</v>
+      </c>
+    </row>
+    <row r="149" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A149" t="s">
+        <v>172</v>
+      </c>
+      <c r="B149">
+        <v>5339511.8662871197</v>
+      </c>
+    </row>
+    <row r="150" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A150" t="s">
+        <v>79</v>
+      </c>
+      <c r="B150">
+        <v>5197731.9613897596</v>
+      </c>
+    </row>
+    <row r="151" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A151" t="s">
+        <v>80</v>
+      </c>
+      <c r="B151">
+        <v>392026.197319019</v>
+      </c>
+    </row>
+    <row r="152" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A152" t="s">
+        <v>81</v>
+      </c>
+      <c r="B152">
+        <v>264152.43364930502</v>
+      </c>
+    </row>
+    <row r="153" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A153" t="s">
+        <v>82</v>
+      </c>
+      <c r="B153">
+        <v>510287.181356752</v>
+      </c>
+    </row>
+    <row r="154" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A154" t="s">
+        <v>128</v>
+      </c>
+      <c r="B154">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="155" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A155" t="s">
+        <v>223</v>
+      </c>
+      <c r="B155">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <sortState ref="A2:B170">
+    <sortCondition ref="A2:A170"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>